<commit_message>
update document Azure A phuong
</commit_message>
<xml_diff>
--- a/Document/Server/Server.xlsx
+++ b/Document/Server/Server.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Linux vs Nginx" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Name</t>
   </si>
@@ -38,13 +39,136 @@
   <si>
     <t>là viết tắt của Content Delivery Network, có thể tạm dịch là mạng phân phối nội dung. Với hệ thống các máy chủ được đặt tại nhiều nơi sẽ giúp tối ưu tốc độ website cho người truy cập, cải thiện chất lượng website.
 CDN giúp các nhà phát triển nội dung, website và ứng dụng có thể đưa những sản phẩm của họ tới khách hàng ở những nơi có khoảng cách xa về địa lý một cách nhanh nhất, thông qua việc truy cập từ những máy chủ ở gần đó.</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>https://phoenixnap.com/kb/how-to-create-add-sudo-user-centos</t>
+  </si>
+  <si>
+    <t>Add user in linux server.</t>
+  </si>
+  <si>
+    <t>The deployment in net core</t>
+  </si>
+  <si>
+    <t>https://docs.microsoft.com/en-us/aspnet/core/host-and-deploy/linux-nginx?view=aspnetcore-3.1&amp;tabs=aspnetcore3x</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Cấu hình.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RUN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : sudo nano /etc/systemd/system/kestrel-helloapp.service
+[Unit]
+Description=Example .NET Web API App running on Ubuntu
+[Service]
+WorkingDirectory=/var/www/helloapp
+ExecStart=/usr/bin/dotnet /var/www/helloapp/helloapp.dll
+Restart=always
+# Restart service after 10 seconds if the dotnet service crashes:
+RestartSec=10
+KillSignal=SIGINT
+SyslogIdentifier=dotnet-example
+User=www-data
+Environment=ASPNETCORE_ENVIRONMENT=Production
+Environment=DOTNET_PRINT_TELEMETRY_MESSAGE=false
+[Install]
+WantedBy=multi-user.target
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RUN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sudo systemctl enable kestrel-helloapp.service: enable service
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RUN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  sudo systemctl start kestrel-helloapp.service : start a service
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>RUN</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> systemctl status kestrel-helloapp.service: view status of service</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,6 +181,22 @@
       <color rgb="FF1D2129"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -76,20 +216,40 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="11">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -122,13 +282,25 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D3" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D3" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
   <autoFilter ref="A2:D3"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="3"/>
-    <tableColumn id="2" name="Desciptions" dataDxfId="2"/>
-    <tableColumn id="3" name="Note" dataDxfId="1"/>
-    <tableColumn id="4" name="Link" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="8"/>
+    <tableColumn id="2" name="Desciptions" dataDxfId="7"/>
+    <tableColumn id="3" name="Note" dataDxfId="6"/>
+    <tableColumn id="4" name="Link" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C17" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="A2:C17"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Name" dataDxfId="4"/>
+    <tableColumn id="2" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" name="Link" dataDxfId="2" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -399,8 +571,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -443,4 +615,102 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="40.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="90.1796875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="69.08984375" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="319" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C5" s="3"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C6" s="3"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C13" s="3"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="C16" s="3"/>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.35">
+      <c r="C17" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C3" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update file excel deploy net core with server nginx
</commit_message>
<xml_diff>
--- a/Document/Server/Server.xlsx
+++ b/Document/Server/Server.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="cdn" sheetId="1" r:id="rId1"/>
     <sheet name="Linux vs Nginx" sheetId="2" r:id="rId2"/>
+    <sheet name="DeployNginx" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Name</t>
   </si>
@@ -163,12 +164,117 @@
       <t xml:space="preserve"> systemctl status kestrel-helloapp.service: view status of service</t>
     </r>
   </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>https://medium.com/@muhamadiqbal2106/how-to-deploy-asp-net-core-to-centos-7-redhat-7a4dcb2b450a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Update kernel.
+Update yum.
+</t>
+  </si>
+  <si>
+    <t>Install net core 3.1</t>
+  </si>
+  <si>
+    <t>Setup Supervisor</t>
+  </si>
+  <si>
+    <t>- yum install epel-release
+- sudo yum install supervisor -y (có thể sử dụng service thay thế supervisor)</t>
+  </si>
+  <si>
+    <t>- sudo yum install dotnet-sdk-3.1
+- sudo yum install aspnetcore-runtime-3.1</t>
+  </si>
+  <si>
+    <t>- sudo yum update -y
+- sudo rpm -Uvh - https://packages.microsoft.com/config/centos/7/packages-microsoft-prod.rpm</t>
+  </si>
+  <si>
+    <t>install Nginx as a reverse proxy</t>
+  </si>
+  <si>
+    <t>- sudo yum install nginx -y</t>
+  </si>
+  <si>
+    <t>- sudo vi /etc/nginx/nginx.conf (setup default)</t>
+  </si>
+  <si>
+    <t>If you publish not in folder www linux</t>
+  </si>
+  <si>
+    <t>Setup firewall rules</t>
+  </si>
+  <si>
+    <t>https://www.digitalocean.com/community/tutorials/how-to-set-up-a-firewall-using-firewalld-on-centos-7</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - sudo firewall-cmd --zone=public  --add-service=http (run time)
+- sudo firewall-cmd --zone=public  --add-service=http --permanent (permanent reboot to effect)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - firewall-cmd --get-default-zone (Lấy zone default).
+ - firewall-cmd --get-services (Lấy thông tin dịch vụ).
+- sudo firewall-cmd --zone=public --add-port=5000/tcp ( runtime Thêm port theo cách cũ thay vì thêm services).
+- sudo firewall-cmd --zone=public --add-port=5000/tcp --permanent ( permanent Thêm port theo cách cũ thay vì thêm services)
+</t>
+  </si>
+  <si>
+    <t>Redis</t>
+  </si>
+  <si>
+    <t>https://www.digitalocean.com/community/tutorials/how-to-install-secure-redis-centos-7</t>
+  </si>
+  <si>
+    <t>client_server_private_IP:127.0.0.1,etc…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- with use Firewall
+- sudo firewall-cmd --permanent --new-zone=redis (create a new zone with name redis)
+- sudo firewall-cmd --permanent --zone=redis --add-port=6379/tcp (set port to use redis with port 6379)
+- sudo firewall-cmd --permanent --zone=redis --add-source={client_server_private_IP} (setup IP private in server linux)
+</t>
+  </si>
+  <si>
+    <t>- Default sẽ lấy locahost và cổng 6379.
+-  Vào /etc/redis.conf thêm password cho redis : requirepass {password}.
+- Sử dụng redis-cli để CLI redis.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">- vi /etc/sysconfig/selinux
+- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>SELINUX=disabled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+sudo shutdown -r now</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -198,6 +304,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -220,7 +339,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -229,12 +348,150 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="18">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -282,25 +539,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D3" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D3" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A2:D3"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="8"/>
-    <tableColumn id="2" name="Desciptions" dataDxfId="7"/>
-    <tableColumn id="3" name="Note" dataDxfId="6"/>
-    <tableColumn id="4" name="Link" dataDxfId="5"/>
+    <tableColumn id="1" name="Name" dataDxfId="15"/>
+    <tableColumn id="2" name="Desciptions" dataDxfId="14"/>
+    <tableColumn id="3" name="Note" dataDxfId="13"/>
+    <tableColumn id="4" name="Link" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C17" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A2:C17"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Name" dataDxfId="4"/>
-    <tableColumn id="2" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" name="Link" dataDxfId="2" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="Name" dataDxfId="9"/>
+    <tableColumn id="2" name="Description" dataDxfId="8"/>
+    <tableColumn id="3" name="Link" dataDxfId="7" dataCellStyle="Hyperlink"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:E9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
+  <autoFilter ref="A2:E9"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="Name" dataDxfId="5"/>
+    <tableColumn id="2" name="Description" dataDxfId="4"/>
+    <tableColumn id="3" name="Example" dataDxfId="3"/>
+    <tableColumn id="4" name="Note" dataDxfId="2"/>
+    <tableColumn id="5" name="Link" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -621,7 +892,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C17"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -713,4 +984,144 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:E9"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="38.6328125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.54296875" style="4" customWidth="1"/>
+    <col min="2" max="2" width="48.90625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="77" style="4" customWidth="1"/>
+    <col min="4" max="4" width="47.7265625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="59.54296875" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="38.6328125" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:5" ht="18" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="70" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="35" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+    </row>
+    <row r="5" spans="1:5" ht="52.5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+    </row>
+    <row r="6" spans="1:5" ht="35" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="1:5" ht="53" x14ac:dyDescent="0.35">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="1:5" ht="140" x14ac:dyDescent="0.35">
+      <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="140" x14ac:dyDescent="0.35">
+      <c r="A9" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E8" r:id="rId2"/>
+    <hyperlink ref="E9" r:id="rId3"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Deploy with signalr nginx
</commit_message>
<xml_diff>
--- a/Document/Server/Server.xlsx
+++ b/Document/Server/Server.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Name</t>
   </si>
@@ -269,12 +269,43 @@
 sudo shutdown -r now</t>
     </r>
   </si>
+  <si>
+    <t>Deploy with signalr nginx</t>
+  </si>
+  <si>
+    <t>server {
+    listen 80;
+    location / {
+        proxy_pass http://localhost:5000;
+        proxy_http_version 1.1;
+        proxy_set_header Upgrade $http_upgrade;
+        proxy_set_header Connection keep-alive;
+        proxy_set_header Host $host;
+        proxy_cache_bypass $http_upgrade;
+    }
+    location /api/chat {
+        proxy_pass http://localhost:5000;
+        proxy_http_version 1.1;
+        proxy_set_header Upgrade $http_upgrade;
+        proxy_set_header Connection "upgrade";
+        proxy_set_header Host $host;
+        proxy_cache_bypass $http_upgrade;
+    }
+}</t>
+  </si>
+  <si>
+    <t>https://medium.com/@alm.ozdmr/deployment-of-signalr-with-nginx-daf392cf2b93</t>
+  </si>
+  <si>
+    <t>Thay đổi location /api/chat mapHub.
+Sử dụng proxy_set_header Connection "upgrade"; with websocket realtime.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,6 +348,11 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -339,7 +375,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -358,6 +394,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -564,14 +603,14 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:E9" totalsRowShown="0" headerRowDxfId="6" dataDxfId="0">
-  <autoFilter ref="A2:E9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:E15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="A2:E15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="5"/>
-    <tableColumn id="2" name="Description" dataDxfId="4"/>
-    <tableColumn id="3" name="Example" dataDxfId="3"/>
-    <tableColumn id="4" name="Note" dataDxfId="2"/>
-    <tableColumn id="5" name="Link" dataDxfId="1"/>
+    <tableColumn id="1" name="Name" dataDxfId="4"/>
+    <tableColumn id="2" name="Description" dataDxfId="3"/>
+    <tableColumn id="3" name="Example" dataDxfId="2"/>
+    <tableColumn id="4" name="Note" dataDxfId="1"/>
+    <tableColumn id="5" name="Link" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -988,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E9"/>
+  <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.6328125" defaultRowHeight="17.5" x14ac:dyDescent="0.35"/>
@@ -1112,16 +1151,67 @@
         <v>29</v>
       </c>
     </row>
+    <row r="10" spans="1:5" ht="332.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="8"/>
+      <c r="E10" s="7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1"/>
     <hyperlink ref="E8" r:id="rId2"/>
     <hyperlink ref="E9" r:id="rId3"/>
+    <hyperlink ref="E10" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
file excel and world about Server linux, google cloudsm acccount, document about isntall Mysql in centos 7
</commit_message>
<xml_diff>
--- a/Document/Server/Server.xlsx
+++ b/Document/Server/Server.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="cdn" sheetId="1" r:id="rId1"/>
     <sheet name="Linux vs Nginx" sheetId="2" r:id="rId2"/>
     <sheet name="DeployNginx" sheetId="3" r:id="rId3"/>
+    <sheet name="syntax linux" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="42">
   <si>
     <t>Name</t>
   </si>
@@ -299,6 +300,18 @@
   <si>
     <t>Thay đổi location /api/chat mapHub.
 Sử dụng proxy_set_header Connection "upgrade"; with websocket realtime.</t>
+  </si>
+  <si>
+    <t>Descriptions</t>
+  </si>
+  <si>
+    <t>Command line</t>
+  </si>
+  <si>
+    <t>netstat -plntu</t>
+  </si>
+  <si>
+    <t>Show active internet connections</t>
   </si>
 </sst>
 </file>
@@ -375,7 +388,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -399,12 +412,33 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
+  <dxfs count="24">
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -578,39 +612,52 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D3" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:D3" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
   <autoFilter ref="A2:D3"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Name" dataDxfId="15"/>
-    <tableColumn id="2" name="Desciptions" dataDxfId="14"/>
-    <tableColumn id="3" name="Note" dataDxfId="13"/>
-    <tableColumn id="4" name="Link" dataDxfId="12"/>
+    <tableColumn id="1" name="Name" dataDxfId="21"/>
+    <tableColumn id="2" name="Desciptions" dataDxfId="20"/>
+    <tableColumn id="3" name="Note" dataDxfId="19"/>
+    <tableColumn id="4" name="Link" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C17" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A2:C17" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <autoFilter ref="A2:C17"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Name" dataDxfId="9"/>
-    <tableColumn id="2" name="Description" dataDxfId="8"/>
-    <tableColumn id="3" name="Link" dataDxfId="7" dataCellStyle="Hyperlink"/>
+    <tableColumn id="1" name="Name" dataDxfId="15"/>
+    <tableColumn id="2" name="Description" dataDxfId="14"/>
+    <tableColumn id="3" name="Link" dataDxfId="13" dataCellStyle="Hyperlink"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:E15" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A2:E15" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A2:E15"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Name" dataDxfId="4"/>
-    <tableColumn id="2" name="Description" dataDxfId="3"/>
-    <tableColumn id="3" name="Example" dataDxfId="2"/>
-    <tableColumn id="4" name="Note" dataDxfId="1"/>
-    <tableColumn id="5" name="Link" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="10"/>
+    <tableColumn id="2" name="Description" dataDxfId="9"/>
+    <tableColumn id="3" name="Example" dataDxfId="8"/>
+    <tableColumn id="4" name="Note" dataDxfId="7"/>
+    <tableColumn id="5" name="Link" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A3:D4" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A3:D4"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="Command line" dataDxfId="5"/>
+    <tableColumn id="2" name="Descriptions" dataDxfId="4"/>
+    <tableColumn id="3" name="Example" dataDxfId="3"/>
+    <tableColumn id="4" name="Link" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1029,7 +1076,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -1214,4 +1261,51 @@
     <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:D4"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="36.7265625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="25.81640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="23" style="9" customWidth="1"/>
+    <col min="4" max="4" width="32.08984375" style="9" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>